<commit_message>
update HKStock add function getHKStockData
</commit_message>
<xml_diff>
--- a/Data/HSC.xlsx
+++ b/Data/HSC.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="275">
   <si>
     <t>ticker</t>
   </si>
@@ -836,6 +836,9 @@
   </si>
   <si>
     <t>2016-08-12</t>
+  </si>
+  <si>
+    <t>2016-08-15</t>
   </si>
 </sst>
 </file>
@@ -1193,7 +1196,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G268"/>
+  <dimension ref="A1:G269"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -7360,6 +7363,29 @@
         <v>13634.97</v>
       </c>
     </row>
+    <row r="269" spans="1:7">
+      <c r="A269" s="1">
+        <v>267</v>
+      </c>
+      <c r="B269" t="s">
+        <v>6</v>
+      </c>
+      <c r="C269" t="s">
+        <v>274</v>
+      </c>
+      <c r="D269">
+        <v>13650.96</v>
+      </c>
+      <c r="E269">
+        <v>13634.97</v>
+      </c>
+      <c r="F269">
+        <v>13757.61</v>
+      </c>
+      <c r="G269">
+        <v>13724</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>